<commit_message>
Code before adding custom leave search and VND language
</commit_message>
<xml_diff>
--- a/public/files/demo_attendance.xlsx
+++ b/public/files/demo_attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSP-PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Affan Ahmed\HRM 3.0 Clone GitHub\HRM-3.0\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9745CA9-9708-4C7B-8B77-B65E5A17E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FCBFC1-5C8D-47C4-AF55-D3082CCA6FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="8">
   <si>
     <t>Check IN Date</t>
   </si>
@@ -42,16 +42,13 @@
     <t>Offdays</t>
   </si>
   <si>
-    <t>sunny</t>
+    <t>EMP NAME</t>
   </si>
   <si>
-    <t>no</t>
+    <t>OFF</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>EMP NAME</t>
+    <t>Employee Name</t>
   </si>
 </sst>
 </file>
@@ -445,7 +442,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,7 +458,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -481,96 +478,88 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6">
-        <v>45682</v>
+        <v>45658</v>
       </c>
       <c r="C2" s="7">
         <v>0.375</v>
       </c>
       <c r="D2" s="6">
-        <v>45682</v>
+        <v>45658</v>
       </c>
       <c r="E2" s="7">
         <v>0.75</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="6">
-        <v>45683</v>
+        <v>45659</v>
       </c>
       <c r="C3" s="7">
         <v>0.375</v>
       </c>
       <c r="D3" s="6">
-        <v>45683</v>
+        <v>45659</v>
       </c>
       <c r="E3" s="7">
         <v>0.75</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6">
-        <v>45684</v>
+        <v>45660</v>
       </c>
       <c r="C4" s="7">
         <v>0.375</v>
       </c>
       <c r="D4" s="6">
-        <v>45684</v>
+        <v>45660</v>
       </c>
       <c r="E4" s="7">
         <v>0.75</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>45685</v>
+        <v>45661</v>
       </c>
       <c r="C5" s="7">
         <v>0.375</v>
       </c>
       <c r="D5" s="6">
-        <v>45685</v>
+        <v>45661</v>
       </c>
       <c r="E5" s="7">
         <v>0.75</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6">
-        <v>45686</v>
+        <v>45662</v>
       </c>
       <c r="C6" s="7">
         <v>0.375</v>
       </c>
       <c r="D6" s="6">
-        <v>45686</v>
+        <v>45662</v>
       </c>
       <c r="E6" s="7">
         <v>0.75</v>
@@ -581,116 +570,106 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="6">
-        <v>45687</v>
+        <v>45663</v>
       </c>
       <c r="C7" s="7">
         <v>0.375</v>
       </c>
       <c r="D7" s="6">
-        <v>45687</v>
+        <v>45663</v>
       </c>
       <c r="E7" s="7">
         <v>0.75</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6">
-        <v>45688</v>
+        <v>45664</v>
       </c>
       <c r="C8" s="7">
         <v>0.375</v>
       </c>
       <c r="D8" s="6">
-        <v>45688</v>
+        <v>45664</v>
       </c>
       <c r="E8" s="7">
         <v>0.75</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>45689</v>
+        <v>45665</v>
       </c>
       <c r="C9" s="7">
         <v>0.375</v>
       </c>
       <c r="D9" s="6">
-        <v>45689</v>
+        <v>45665</v>
       </c>
       <c r="E9" s="7">
         <v>0.75</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10" s="6">
-        <v>45690</v>
+        <v>45666</v>
       </c>
       <c r="C10" s="7">
         <v>0.375</v>
       </c>
       <c r="D10" s="6">
-        <v>45690</v>
+        <v>45666</v>
       </c>
       <c r="E10" s="7">
         <v>0.75</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" s="6">
-        <v>45691</v>
+        <v>45667</v>
       </c>
       <c r="C11" s="7">
         <v>0.375</v>
       </c>
       <c r="D11" s="6">
-        <v>45691</v>
+        <v>45667</v>
       </c>
       <c r="E11" s="7">
         <v>0.75</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12" s="6">
-        <v>45692</v>
+        <v>45668</v>
       </c>
       <c r="C12" s="7">
         <v>0.375</v>
       </c>
       <c r="D12" s="6">
-        <v>45692</v>
+        <v>45668</v>
       </c>
       <c r="E12" s="7">
         <v>0.75</v>
@@ -701,156 +680,142 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B13" s="6">
-        <v>45693</v>
+        <v>45669</v>
       </c>
       <c r="C13" s="7">
         <v>0.375</v>
       </c>
       <c r="D13" s="6">
-        <v>45693</v>
+        <v>45669</v>
       </c>
       <c r="E13" s="7">
         <v>0.75</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B14" s="6">
-        <v>45694</v>
+        <v>45670</v>
       </c>
       <c r="C14" s="7">
         <v>0.375</v>
       </c>
       <c r="D14" s="6">
-        <v>45694</v>
+        <v>45670</v>
       </c>
       <c r="E14" s="7">
         <v>0.75</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B15" s="6">
-        <v>45695</v>
+        <v>45671</v>
       </c>
       <c r="C15" s="7">
         <v>0.375</v>
       </c>
       <c r="D15" s="6">
-        <v>45695</v>
+        <v>45671</v>
       </c>
       <c r="E15" s="7">
         <v>0.75</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B16" s="6">
-        <v>45696</v>
+        <v>45672</v>
       </c>
       <c r="C16" s="7">
         <v>0.375</v>
       </c>
       <c r="D16" s="6">
-        <v>45696</v>
+        <v>45672</v>
       </c>
       <c r="E16" s="7">
         <v>0.75</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17" s="6">
-        <v>45697</v>
+        <v>45673</v>
       </c>
       <c r="C17" s="7">
         <v>0.375</v>
       </c>
       <c r="D17" s="6">
-        <v>45697</v>
+        <v>45673</v>
       </c>
       <c r="E17" s="7">
         <v>0.75</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B18" s="6">
-        <v>45698</v>
+        <v>45674</v>
       </c>
       <c r="C18" s="7">
         <v>0.375</v>
       </c>
       <c r="D18" s="6">
-        <v>45698</v>
+        <v>45674</v>
       </c>
       <c r="E18" s="7">
         <v>0.75</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B19" s="6">
-        <v>45699</v>
+        <v>45675</v>
       </c>
       <c r="C19" s="7">
         <v>0.375</v>
       </c>
       <c r="D19" s="6">
-        <v>45699</v>
+        <v>45675</v>
       </c>
       <c r="E19" s="7">
         <v>0.75</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B20" s="6">
-        <v>45700</v>
+        <v>45676</v>
       </c>
       <c r="C20" s="7">
         <v>0.375</v>
       </c>
       <c r="D20" s="6">
-        <v>45700</v>
+        <v>45676</v>
       </c>
       <c r="E20" s="7">
         <v>0.75</v>
@@ -861,176 +826,160 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B21" s="6">
-        <v>45701</v>
+        <v>45677</v>
       </c>
       <c r="C21" s="7">
         <v>0.375</v>
       </c>
       <c r="D21" s="6">
-        <v>45701</v>
+        <v>45677</v>
       </c>
       <c r="E21" s="7">
         <v>0.75</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B22" s="6">
-        <v>45702</v>
+        <v>45678</v>
       </c>
       <c r="C22" s="7">
         <v>0.375</v>
       </c>
       <c r="D22" s="6">
-        <v>45702</v>
+        <v>45678</v>
       </c>
       <c r="E22" s="7">
         <v>0.75</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B23" s="6">
-        <v>45703</v>
+        <v>45679</v>
       </c>
       <c r="C23" s="7">
         <v>0.375</v>
       </c>
       <c r="D23" s="6">
-        <v>45703</v>
+        <v>45679</v>
       </c>
       <c r="E23" s="7">
         <v>0.75</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6">
-        <v>45704</v>
+        <v>45680</v>
       </c>
       <c r="C24" s="7">
         <v>0.375</v>
       </c>
       <c r="D24" s="6">
-        <v>45704</v>
+        <v>45680</v>
       </c>
       <c r="E24" s="7">
         <v>0.75</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B25" s="6">
-        <v>45705</v>
+        <v>45681</v>
       </c>
       <c r="C25" s="7">
         <v>0.375</v>
       </c>
       <c r="D25" s="6">
-        <v>45705</v>
+        <v>45681</v>
       </c>
       <c r="E25" s="7">
         <v>0.75</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B26" s="6">
-        <v>45706</v>
+        <v>45682</v>
       </c>
       <c r="C26" s="7">
         <v>0.375</v>
       </c>
       <c r="D26" s="6">
-        <v>45706</v>
+        <v>45682</v>
       </c>
       <c r="E26" s="7">
         <v>0.75</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B27" s="6">
-        <v>45707</v>
+        <v>45683</v>
       </c>
       <c r="C27" s="7">
         <v>0.375</v>
       </c>
       <c r="D27" s="6">
-        <v>45707</v>
+        <v>45683</v>
       </c>
       <c r="E27" s="7">
         <v>0.75</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B28" s="6">
-        <v>45708</v>
+        <v>45684</v>
       </c>
       <c r="C28" s="7">
         <v>0.375</v>
       </c>
       <c r="D28" s="6">
-        <v>45708</v>
+        <v>45684</v>
       </c>
       <c r="E28" s="7">
         <v>0.75</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B29" s="6">
-        <v>45709</v>
+        <v>45685</v>
       </c>
       <c r="C29" s="7">
         <v>0.375</v>
       </c>
       <c r="D29" s="6">
-        <v>45709</v>
+        <v>45685</v>
       </c>
       <c r="E29" s="7">
         <v>0.75</v>
@@ -1041,63 +990,57 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B30" s="6">
-        <v>45710</v>
+        <v>45686</v>
       </c>
       <c r="C30" s="7">
         <v>0.375</v>
       </c>
       <c r="D30" s="6">
-        <v>45710</v>
+        <v>45686</v>
       </c>
       <c r="E30" s="7">
         <v>0.75</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B31" s="6">
-        <v>45711</v>
+        <v>45687</v>
       </c>
       <c r="C31" s="7">
         <v>0.375</v>
       </c>
       <c r="D31" s="6">
-        <v>45711</v>
+        <v>45687</v>
       </c>
       <c r="E31" s="7">
         <v>0.75</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B32" s="6">
-        <v>45712</v>
+        <v>45688</v>
       </c>
       <c r="C32" s="7">
         <v>0.375</v>
       </c>
       <c r="D32" s="6">
-        <v>45712</v>
+        <v>45688</v>
       </c>
       <c r="E32" s="7">
         <v>0.75</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="F32" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>